<commit_message>
Updated version of annotations
</commit_message>
<xml_diff>
--- a/result/Annotations_GroupE.xlsx
+++ b/result/Annotations_GroupE.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29721"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29816"/>
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,9 +9,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ituniversity-my.sharepoint.com/personal/vkap_itu_dk/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="720" documentId="8_{74F08C27-E9B4-3F4A-8F60-87D64CECE72E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9CBD79D7-4DCF-431F-99E3-5FF76D3F0DDF}"/>
+  <xr:revisionPtr revIDLastSave="1212" documentId="8_{74F08C27-E9B4-3F4A-8F60-87D64CECE72E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68F975D3-F6B1-44E7-BC6C-12DE96716BBD}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{672A4043-0214-1843-B5FB-4017F37BC401}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="15880" xr2:uid="{672A4043-0214-1843-B5FB-4017F37BC401}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="134">
   <si>
     <t>Image_id</t>
   </si>
@@ -75,12 +75,24 @@
     <t>Comments:  Annotator names:   A1 = Andreea, A2 = Shayan,  A3 = Victoria S, A4 = Victoria K, A5 = Wladimir</t>
   </si>
   <si>
+    <t>Average hair</t>
+  </si>
+  <si>
+    <t>Average pen marks</t>
+  </si>
+  <si>
     <t>PAT_14_22_850.png</t>
   </si>
   <si>
+    <t>Everyone in the group worked on this file with annotations but it will be uploaded on github by a single person.</t>
+  </si>
+  <si>
     <t>PAT_20_30_44.png</t>
   </si>
   <si>
+    <t>You can see the changes made by each person in the Review -&gt; Changes in history</t>
+  </si>
+  <si>
     <t>PAT_44_63_151.png</t>
   </si>
   <si>
@@ -424,6 +436,9 @@
   </si>
   <si>
     <t>PAT_2125_4653_497.png</t>
+  </si>
+  <si>
+    <t>TOTAL AVERAGES:</t>
   </si>
 </sst>
 </file>
@@ -439,12 +454,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -459,8 +486,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -795,10 +824,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E9A3E64-F21A-8341-B7F8-B2DDA04EDB3C}">
-  <dimension ref="A1:L118"/>
+  <dimension ref="A1:N119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
@@ -812,10 +841,11 @@
     <col min="7" max="7" width="15.625" customWidth="1"/>
     <col min="8" max="9" width="15.5" customWidth="1"/>
     <col min="11" max="11" width="16.375" customWidth="1"/>
-    <col min="12" max="12" width="85.125" customWidth="1"/>
+    <col min="12" max="12" width="87.125" customWidth="1"/>
+    <col min="14" max="14" width="15.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -852,10 +882,22 @@
       <c r="L1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -866,6 +908,12 @@
       <c r="F2">
         <v>0</v>
       </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
       <c r="I2">
         <v>0</v>
       </c>
@@ -875,10 +923,27 @@
       <c r="K2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="L2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2">
+        <f>AVERAGE(B2:F2)</f>
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <f>ROUND(AVERAGE(G2:K2),2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -889,6 +954,12 @@
       <c r="F3">
         <v>2</v>
       </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
       <c r="I3">
         <v>1</v>
       </c>
@@ -898,10 +969,27 @@
       <c r="K3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="L3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3">
+        <f>ROUND(AVERAGE(B3:F3),2)</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N66" si="0">ROUND(AVERAGE(G3:K3),2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>18</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -912,6 +1000,12 @@
       <c r="F4">
         <v>1</v>
       </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
       <c r="I4">
         <v>1</v>
       </c>
@@ -921,10 +1015,24 @@
       <c r="K4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="M4">
+        <f t="shared" ref="M4:M67" si="1">ROUND(AVERAGE(B4:F4),2)</f>
+        <v>1.6</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>19</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -935,6 +1043,12 @@
       <c r="F5">
         <v>2</v>
       </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
       <c r="I5">
         <v>0</v>
       </c>
@@ -944,10 +1058,24 @@
       <c r="K5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="M5">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -958,6 +1086,12 @@
       <c r="F6">
         <v>0</v>
       </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
       <c r="I6">
         <v>0</v>
       </c>
@@ -967,10 +1101,24 @@
       <c r="K6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="M6">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -981,6 +1129,12 @@
       <c r="F7">
         <v>2</v>
       </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
       <c r="I7">
         <v>1</v>
       </c>
@@ -990,10 +1144,24 @@
       <c r="K7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="M7">
+        <f t="shared" si="1"/>
+        <v>2.4</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>22</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1004,6 +1172,12 @@
       <c r="F8">
         <v>0</v>
       </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
       <c r="I8">
         <v>0</v>
       </c>
@@ -1013,10 +1187,24 @@
       <c r="K8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="M8">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>23</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
       </c>
       <c r="D9">
         <v>3</v>
@@ -1027,6 +1215,12 @@
       <c r="F9">
         <v>3</v>
       </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
       <c r="I9">
         <v>1</v>
       </c>
@@ -1036,10 +1230,24 @@
       <c r="K9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="M9">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>24</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1050,6 +1258,12 @@
       <c r="F10">
         <v>0</v>
       </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
       <c r="I10">
         <v>0</v>
       </c>
@@ -1059,10 +1273,24 @@
       <c r="K10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="M10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>25</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
       </c>
       <c r="D11">
         <v>3</v>
@@ -1073,6 +1301,12 @@
       <c r="F11">
         <v>3</v>
       </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
       <c r="I11">
         <v>1</v>
       </c>
@@ -1082,10 +1316,24 @@
       <c r="K11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="M11">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>26</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -1096,6 +1344,12 @@
       <c r="F12">
         <v>0</v>
       </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
       <c r="I12">
         <v>1</v>
       </c>
@@ -1105,10 +1359,24 @@
       <c r="K12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="M12">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>27</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
       </c>
       <c r="D13">
         <v>2</v>
@@ -1119,6 +1387,12 @@
       <c r="F13">
         <v>0</v>
       </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
       <c r="I13">
         <v>1</v>
       </c>
@@ -1128,10 +1402,24 @@
       <c r="K13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="M13">
+        <f t="shared" si="1"/>
+        <v>1.4</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>28</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -1142,6 +1430,12 @@
       <c r="F14">
         <v>0</v>
       </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
       <c r="I14">
         <v>0</v>
       </c>
@@ -1151,10 +1445,24 @@
       <c r="K14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="M14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>29</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -1165,6 +1473,12 @@
       <c r="F15">
         <v>0</v>
       </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
       <c r="I15">
         <v>0</v>
       </c>
@@ -1174,10 +1488,24 @@
       <c r="K15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="M15">
+        <f t="shared" si="1"/>
+        <v>0.4</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>30</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -1188,6 +1516,12 @@
       <c r="F16">
         <v>1</v>
       </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
       <c r="I16">
         <v>0</v>
       </c>
@@ -1197,10 +1531,24 @@
       <c r="K16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:11">
+      <c r="M16">
+        <f t="shared" si="1"/>
+        <v>1.6</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1211,6 +1559,12 @@
       <c r="F17">
         <v>0</v>
       </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
       <c r="I17">
         <v>1</v>
       </c>
@@ -1220,10 +1574,24 @@
       <c r="K17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:11">
+      <c r="M17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>32</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
       </c>
       <c r="D18">
         <v>2</v>
@@ -1234,6 +1602,12 @@
       <c r="F18">
         <v>1</v>
       </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
       <c r="I18">
         <v>0</v>
       </c>
@@ -1243,10 +1617,24 @@
       <c r="K18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:11">
+      <c r="M18">
+        <f t="shared" si="1"/>
+        <v>1.2</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>33</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -1257,6 +1645,12 @@
       <c r="F19">
         <v>0</v>
       </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
       <c r="I19">
         <v>0</v>
       </c>
@@ -1266,10 +1660,24 @@
       <c r="K19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:11">
+      <c r="M19">
+        <f t="shared" si="1"/>
+        <v>0.4</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>34</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
       </c>
       <c r="D20">
         <v>3</v>
@@ -1280,6 +1688,12 @@
       <c r="F20">
         <v>1</v>
       </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
       <c r="I20">
         <v>1</v>
       </c>
@@ -1289,10 +1703,24 @@
       <c r="K20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:11">
+      <c r="M20">
+        <f t="shared" si="1"/>
+        <v>1.8</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>35</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
       </c>
       <c r="D21">
         <v>2</v>
@@ -1303,6 +1731,12 @@
       <c r="F21">
         <v>0</v>
       </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
       <c r="I21">
         <v>0</v>
       </c>
@@ -1312,10 +1746,24 @@
       <c r="K21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:11">
+      <c r="M21">
+        <f t="shared" si="1"/>
+        <v>0.4</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>36</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -1326,6 +1774,12 @@
       <c r="F22">
         <v>0</v>
       </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
       <c r="I22">
         <v>0</v>
       </c>
@@ -1335,10 +1789,24 @@
       <c r="K22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:11">
+      <c r="M22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>37</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
       </c>
       <c r="D23">
         <v>3</v>
@@ -1349,6 +1817,12 @@
       <c r="F23">
         <v>1</v>
       </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
       <c r="I23">
         <v>1</v>
       </c>
@@ -1358,10 +1832,24 @@
       <c r="K23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:11">
+      <c r="M23">
+        <f t="shared" si="1"/>
+        <v>1.4</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>38</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -1372,6 +1860,12 @@
       <c r="F24">
         <v>0</v>
       </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
       <c r="I24">
         <v>0</v>
       </c>
@@ -1381,10 +1875,24 @@
       <c r="K24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:11">
+      <c r="M24">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>39</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
       </c>
       <c r="D25">
         <v>2</v>
@@ -1395,6 +1903,12 @@
       <c r="F25">
         <v>1</v>
       </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
       <c r="I25">
         <v>0</v>
       </c>
@@ -1404,10 +1918,24 @@
       <c r="K25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:11">
+      <c r="M25">
+        <f t="shared" si="1"/>
+        <v>1.8</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>40</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -1418,6 +1946,12 @@
       <c r="F26">
         <v>2</v>
       </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
       <c r="I26">
         <v>0</v>
       </c>
@@ -1427,10 +1961,24 @@
       <c r="K26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:11">
+      <c r="M26">
+        <f t="shared" si="1"/>
+        <v>1.2</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>41</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -1441,6 +1989,12 @@
       <c r="F27">
         <v>0</v>
       </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
       <c r="I27">
         <v>0</v>
       </c>
@@ -1450,10 +2004,24 @@
       <c r="K27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:11">
+      <c r="M27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
       <c r="A28" t="s">
-        <v>38</v>
+        <v>42</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -1464,6 +2032,12 @@
       <c r="F28">
         <v>1</v>
       </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
       <c r="I28">
         <v>0</v>
       </c>
@@ -1473,10 +2047,24 @@
       <c r="K28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:11">
+      <c r="M28">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>43</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -1487,6 +2075,12 @@
       <c r="F29">
         <v>1</v>
       </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
       <c r="I29">
         <v>0</v>
       </c>
@@ -1496,10 +2090,24 @@
       <c r="K29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:11">
+      <c r="M29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
       <c r="A30" t="s">
-        <v>40</v>
+        <v>44</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -1510,6 +2118,12 @@
       <c r="F30">
         <v>1</v>
       </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
       <c r="I30">
         <v>1</v>
       </c>
@@ -1519,10 +2133,24 @@
       <c r="K30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:11">
+      <c r="M30">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
       <c r="A31" t="s">
-        <v>41</v>
+        <v>45</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -1533,6 +2161,12 @@
       <c r="F31">
         <v>2</v>
       </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
       <c r="I31">
         <v>0</v>
       </c>
@@ -1542,10 +2176,24 @@
       <c r="K31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:11">
+      <c r="M31">
+        <f t="shared" si="1"/>
+        <v>1.6</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
       <c r="A32" t="s">
-        <v>42</v>
+        <v>46</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32">
+        <v>3</v>
       </c>
       <c r="D32">
         <v>3</v>
@@ -1556,6 +2204,12 @@
       <c r="F32">
         <v>3</v>
       </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
       <c r="I32">
         <v>0</v>
       </c>
@@ -1565,10 +2219,24 @@
       <c r="K32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:11">
+      <c r="M32">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
       <c r="A33" t="s">
-        <v>43</v>
+        <v>47</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -1579,6 +2247,12 @@
       <c r="F33">
         <v>0</v>
       </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
       <c r="I33">
         <v>0</v>
       </c>
@@ -1588,10 +2262,24 @@
       <c r="K33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:11">
+      <c r="M33">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
       <c r="A34" t="s">
-        <v>44</v>
+        <v>48</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
       </c>
       <c r="D34">
         <v>2</v>
@@ -1602,6 +2290,12 @@
       <c r="F34">
         <v>0</v>
       </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
       <c r="I34">
         <v>0</v>
       </c>
@@ -1611,10 +2305,24 @@
       <c r="K34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:11">
+      <c r="M34">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
       <c r="A35" t="s">
-        <v>45</v>
+        <v>49</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -1625,6 +2333,12 @@
       <c r="F35">
         <v>0</v>
       </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
       <c r="I35">
         <v>0</v>
       </c>
@@ -1634,10 +2348,24 @@
       <c r="K35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:11">
+      <c r="M35">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
       <c r="A36" t="s">
-        <v>46</v>
+        <v>50</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
       </c>
       <c r="D36">
         <v>2</v>
@@ -1648,6 +2376,12 @@
       <c r="F36">
         <v>2</v>
       </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
       <c r="I36">
         <v>0</v>
       </c>
@@ -1657,10 +2391,24 @@
       <c r="K36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:11">
+      <c r="M36">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
       <c r="A37" t="s">
-        <v>47</v>
+        <v>51</v>
+      </c>
+      <c r="B37">
+        <v>3</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
       </c>
       <c r="D37">
         <v>3</v>
@@ -1671,6 +2419,12 @@
       <c r="F37">
         <v>3</v>
       </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
       <c r="I37">
         <v>0</v>
       </c>
@@ -1680,10 +2434,24 @@
       <c r="K37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:11">
+      <c r="M37">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
       <c r="A38" t="s">
-        <v>48</v>
+        <v>52</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
       </c>
       <c r="D38">
         <v>0</v>
@@ -1694,6 +2462,12 @@
       <c r="F38">
         <v>0</v>
       </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
       <c r="I38">
         <v>0</v>
       </c>
@@ -1703,10 +2477,24 @@
       <c r="K38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:11">
+      <c r="M38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
       <c r="A39" t="s">
-        <v>49</v>
+        <v>53</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
       </c>
       <c r="D39">
         <v>0</v>
@@ -1717,6 +2505,12 @@
       <c r="F39">
         <v>0</v>
       </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
       <c r="I39">
         <v>0</v>
       </c>
@@ -1726,10 +2520,24 @@
       <c r="K39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:11">
+      <c r="M39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
       <c r="A40" t="s">
-        <v>50</v>
+        <v>54</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -1740,6 +2548,12 @@
       <c r="F40">
         <v>0</v>
       </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
       <c r="I40">
         <v>1</v>
       </c>
@@ -1749,10 +2563,24 @@
       <c r="K40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:11">
+      <c r="M40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
       <c r="A41" t="s">
-        <v>51</v>
+        <v>55</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
       </c>
       <c r="D41">
         <v>2</v>
@@ -1763,6 +2591,12 @@
       <c r="F41">
         <v>2</v>
       </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
       <c r="I41">
         <v>1</v>
       </c>
@@ -1772,10 +2606,24 @@
       <c r="K41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:11">
+      <c r="M41">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="N41">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
       <c r="A42" t="s">
-        <v>52</v>
+        <v>56</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -1786,6 +2634,12 @@
       <c r="F42">
         <v>0</v>
       </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
       <c r="I42">
         <v>0</v>
       </c>
@@ -1795,10 +2649,24 @@
       <c r="K42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:11">
+      <c r="M42">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N42">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
       <c r="A43" t="s">
-        <v>53</v>
+        <v>57</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -1809,6 +2677,12 @@
       <c r="F43">
         <v>0</v>
       </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
       <c r="I43">
         <v>0</v>
       </c>
@@ -1818,10 +2692,24 @@
       <c r="K43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:11">
+      <c r="M43">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="N43">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
       <c r="A44" t="s">
-        <v>54</v>
+        <v>58</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -1832,6 +2720,12 @@
       <c r="F44">
         <v>0</v>
       </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
       <c r="I44">
         <v>0</v>
       </c>
@@ -1841,10 +2735,24 @@
       <c r="K44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:11">
+      <c r="M44">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="N44">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
       <c r="A45" t="s">
-        <v>55</v>
+        <v>59</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
       </c>
       <c r="D45">
         <v>0</v>
@@ -1855,6 +2763,12 @@
       <c r="F45">
         <v>0</v>
       </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
       <c r="I45">
         <v>0</v>
       </c>
@@ -1864,10 +2778,24 @@
       <c r="K45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:11">
+      <c r="M45">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N45">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14">
       <c r="A46" t="s">
-        <v>56</v>
+        <v>60</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
       </c>
       <c r="D46">
         <v>1</v>
@@ -1878,6 +2806,12 @@
       <c r="F46">
         <v>1</v>
       </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
       <c r="I46">
         <v>0</v>
       </c>
@@ -1887,10 +2821,24 @@
       <c r="K46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:11">
+      <c r="M46">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N46">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14">
       <c r="A47" t="s">
-        <v>57</v>
+        <v>61</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
       </c>
       <c r="D47">
         <v>1</v>
@@ -1901,6 +2849,12 @@
       <c r="F47">
         <v>0</v>
       </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
       <c r="I47">
         <v>0</v>
       </c>
@@ -1910,10 +2864,24 @@
       <c r="K47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:11">
+      <c r="M47">
+        <f t="shared" si="1"/>
+        <v>0.6</v>
+      </c>
+      <c r="N47">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14">
       <c r="A48" t="s">
-        <v>58</v>
+        <v>62</v>
+      </c>
+      <c r="B48">
+        <v>2</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
       </c>
       <c r="D48">
         <v>2</v>
@@ -1924,6 +2892,12 @@
       <c r="F48">
         <v>2</v>
       </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
       <c r="I48">
         <v>0</v>
       </c>
@@ -1933,10 +2907,24 @@
       <c r="K48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:11">
+      <c r="M48">
+        <f t="shared" si="1"/>
+        <v>1.6</v>
+      </c>
+      <c r="N48">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14">
       <c r="A49" t="s">
-        <v>59</v>
+        <v>63</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -1947,6 +2935,12 @@
       <c r="F49">
         <v>1</v>
       </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
       <c r="I49">
         <v>0</v>
       </c>
@@ -1956,10 +2950,24 @@
       <c r="K49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:11">
+      <c r="M49">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N49">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14">
       <c r="A50" t="s">
-        <v>60</v>
+        <v>64</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
       </c>
       <c r="D50">
         <v>1</v>
@@ -1970,6 +2978,12 @@
       <c r="F50">
         <v>1</v>
       </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
       <c r="I50">
         <v>0</v>
       </c>
@@ -1979,10 +2993,24 @@
       <c r="K50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:11">
+      <c r="M50">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N50">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14">
       <c r="A51" t="s">
-        <v>61</v>
+        <v>65</v>
+      </c>
+      <c r="B51">
+        <v>2</v>
+      </c>
+      <c r="C51">
+        <v>2</v>
       </c>
       <c r="D51">
         <v>2</v>
@@ -1993,6 +3021,12 @@
       <c r="F51">
         <v>2</v>
       </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
       <c r="I51">
         <v>0</v>
       </c>
@@ -2002,10 +3036,24 @@
       <c r="K51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:11">
+      <c r="M51">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="N51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14">
       <c r="A52" t="s">
-        <v>62</v>
+        <v>66</v>
+      </c>
+      <c r="B52">
+        <v>2</v>
+      </c>
+      <c r="C52">
+        <v>2</v>
       </c>
       <c r="D52">
         <v>2</v>
@@ -2016,6 +3064,12 @@
       <c r="F52">
         <v>3</v>
       </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
       <c r="I52">
         <v>0</v>
       </c>
@@ -2025,10 +3079,24 @@
       <c r="K52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:11">
+      <c r="M52">
+        <f t="shared" si="1"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="N52">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14">
       <c r="A53" t="s">
-        <v>63</v>
+        <v>67</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
       </c>
       <c r="D53">
         <v>1</v>
@@ -2039,6 +3107,12 @@
       <c r="F53">
         <v>0</v>
       </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>0</v>
+      </c>
       <c r="I53">
         <v>0</v>
       </c>
@@ -2048,10 +3122,24 @@
       <c r="K53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:11">
+      <c r="M53">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="N53">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14">
       <c r="A54" t="s">
-        <v>64</v>
+        <v>68</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
       </c>
       <c r="D54">
         <v>1</v>
@@ -2062,6 +3150,12 @@
       <c r="F54">
         <v>1</v>
       </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
       <c r="I54">
         <v>0</v>
       </c>
@@ -2071,10 +3165,24 @@
       <c r="K54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:11">
+      <c r="M54">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N54">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14">
       <c r="A55" t="s">
-        <v>65</v>
+        <v>69</v>
+      </c>
+      <c r="B55">
+        <v>0</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
       </c>
       <c r="D55">
         <v>0</v>
@@ -2085,6 +3193,12 @@
       <c r="F55">
         <v>0</v>
       </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
       <c r="I55">
         <v>0</v>
       </c>
@@ -2094,10 +3208,24 @@
       <c r="K55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:11">
+      <c r="M55">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N55">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14">
       <c r="A56" t="s">
-        <v>66</v>
+        <v>70</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
       </c>
       <c r="D56">
         <v>1</v>
@@ -2108,6 +3236,12 @@
       <c r="F56">
         <v>0</v>
       </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <v>1</v>
+      </c>
       <c r="I56">
         <v>1</v>
       </c>
@@ -2117,10 +3251,24 @@
       <c r="K56">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:11">
+      <c r="M56">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="N56">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14">
       <c r="A57" t="s">
-        <v>67</v>
+        <v>71</v>
+      </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -2131,6 +3279,12 @@
       <c r="F57">
         <v>0</v>
       </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
       <c r="I57">
         <v>0</v>
       </c>
@@ -2140,10 +3294,24 @@
       <c r="K57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:11">
+      <c r="M57">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N57">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14">
       <c r="A58" t="s">
-        <v>68</v>
+        <v>72</v>
+      </c>
+      <c r="B58">
+        <v>3</v>
+      </c>
+      <c r="C58">
+        <v>2</v>
       </c>
       <c r="D58">
         <v>3</v>
@@ -2154,6 +3322,12 @@
       <c r="F58">
         <v>3</v>
       </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
       <c r="I58">
         <v>0</v>
       </c>
@@ -2163,10 +3337,24 @@
       <c r="K58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:11">
+      <c r="M58">
+        <f t="shared" si="1"/>
+        <v>2.8</v>
+      </c>
+      <c r="N58">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14">
       <c r="A59" t="s">
-        <v>69</v>
+        <v>73</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -2177,6 +3365,12 @@
       <c r="F59">
         <v>0</v>
       </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
       <c r="I59">
         <v>0</v>
       </c>
@@ -2186,10 +3380,24 @@
       <c r="K59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:11">
+      <c r="M59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14">
       <c r="A60" t="s">
-        <v>70</v>
+        <v>74</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
       </c>
       <c r="D60">
         <v>0</v>
@@ -2200,6 +3408,12 @@
       <c r="F60">
         <v>0</v>
       </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
       <c r="I60">
         <v>0</v>
       </c>
@@ -2209,10 +3423,24 @@
       <c r="K60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:11">
+      <c r="M60">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N60">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14">
       <c r="A61" t="s">
-        <v>71</v>
+        <v>75</v>
+      </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
       </c>
       <c r="D61">
         <v>1</v>
@@ -2223,6 +3451,12 @@
       <c r="F61">
         <v>0</v>
       </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
       <c r="I61">
         <v>0</v>
       </c>
@@ -2232,10 +3466,24 @@
       <c r="K61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:11">
+      <c r="M61">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="N61">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14">
       <c r="A62" t="s">
-        <v>72</v>
+        <v>76</v>
+      </c>
+      <c r="B62">
+        <v>0</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -2246,6 +3494,12 @@
       <c r="F62">
         <v>0</v>
       </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+      <c r="H62">
+        <v>0</v>
+      </c>
       <c r="I62">
         <v>0</v>
       </c>
@@ -2255,10 +3509,24 @@
       <c r="K62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:11">
+      <c r="M62">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N62">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14">
       <c r="A63" t="s">
-        <v>73</v>
+        <v>77</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
       </c>
       <c r="D63">
         <v>1</v>
@@ -2269,6 +3537,12 @@
       <c r="F63">
         <v>0</v>
       </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
       <c r="I63">
         <v>0</v>
       </c>
@@ -2278,10 +3552,24 @@
       <c r="K63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:11">
+      <c r="M63">
+        <f t="shared" si="1"/>
+        <v>0.6</v>
+      </c>
+      <c r="N63">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14">
       <c r="A64" t="s">
-        <v>74</v>
+        <v>78</v>
+      </c>
+      <c r="B64">
+        <v>2</v>
+      </c>
+      <c r="C64">
+        <v>2</v>
       </c>
       <c r="D64">
         <v>2</v>
@@ -2292,6 +3580,12 @@
       <c r="F64">
         <v>1</v>
       </c>
+      <c r="G64">
+        <v>1</v>
+      </c>
+      <c r="H64">
+        <v>1</v>
+      </c>
       <c r="I64">
         <v>1</v>
       </c>
@@ -2301,10 +3595,24 @@
       <c r="K64">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:11">
+      <c r="M64">
+        <f t="shared" si="1"/>
+        <v>1.8</v>
+      </c>
+      <c r="N64">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14">
       <c r="A65" t="s">
-        <v>75</v>
+        <v>79</v>
+      </c>
+      <c r="B65">
+        <v>0</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
       </c>
       <c r="D65">
         <v>0</v>
@@ -2315,6 +3623,12 @@
       <c r="F65">
         <v>0</v>
       </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
       <c r="I65">
         <v>0</v>
       </c>
@@ -2324,10 +3638,24 @@
       <c r="K65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:11">
+      <c r="M65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N65">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14">
       <c r="A66" t="s">
-        <v>76</v>
+        <v>80</v>
+      </c>
+      <c r="B66">
+        <v>3</v>
+      </c>
+      <c r="C66">
+        <v>3</v>
       </c>
       <c r="D66">
         <v>3</v>
@@ -2338,6 +3666,12 @@
       <c r="F66">
         <v>3</v>
       </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+      <c r="H66">
+        <v>0</v>
+      </c>
       <c r="I66">
         <v>0</v>
       </c>
@@ -2347,10 +3681,24 @@
       <c r="K66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:11">
+      <c r="M66">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="N66">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14">
       <c r="A67" t="s">
-        <v>77</v>
+        <v>81</v>
+      </c>
+      <c r="B67">
+        <v>1</v>
+      </c>
+      <c r="C67">
+        <v>1</v>
       </c>
       <c r="D67">
         <v>1</v>
@@ -2361,6 +3709,12 @@
       <c r="F67">
         <v>0</v>
       </c>
+      <c r="G67">
+        <v>1</v>
+      </c>
+      <c r="H67">
+        <v>1</v>
+      </c>
       <c r="I67">
         <v>0</v>
       </c>
@@ -2370,10 +3724,24 @@
       <c r="K67">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:11">
+      <c r="M67">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="N67">
+        <f t="shared" ref="N67:N118" si="2">ROUND(AVERAGE(G67:K67),2)</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14">
       <c r="A68" t="s">
-        <v>78</v>
+        <v>82</v>
+      </c>
+      <c r="B68">
+        <v>0</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
       </c>
       <c r="D68">
         <v>0</v>
@@ -2384,6 +3752,12 @@
       <c r="F68">
         <v>0</v>
       </c>
+      <c r="G68">
+        <v>0</v>
+      </c>
+      <c r="H68">
+        <v>0</v>
+      </c>
       <c r="I68">
         <v>0</v>
       </c>
@@ -2393,10 +3767,24 @@
       <c r="K68">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:11">
+      <c r="M68">
+        <f t="shared" ref="M68:M118" si="3">ROUND(AVERAGE(B68:F68),2)</f>
+        <v>0</v>
+      </c>
+      <c r="N68">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14">
       <c r="A69" t="s">
-        <v>79</v>
+        <v>83</v>
+      </c>
+      <c r="B69">
+        <v>0</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
       </c>
       <c r="D69">
         <v>0</v>
@@ -2407,6 +3795,12 @@
       <c r="F69">
         <v>0</v>
       </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+      <c r="H69">
+        <v>0</v>
+      </c>
       <c r="I69">
         <v>0</v>
       </c>
@@ -2416,10 +3810,24 @@
       <c r="K69">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:11">
+      <c r="M69">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N69">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14">
       <c r="A70" t="s">
-        <v>80</v>
+        <v>84</v>
+      </c>
+      <c r="B70">
+        <v>0</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
       </c>
       <c r="D70">
         <v>0</v>
@@ -2430,6 +3838,12 @@
       <c r="F70">
         <v>0</v>
       </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
       <c r="I70">
         <v>0</v>
       </c>
@@ -2439,10 +3853,24 @@
       <c r="K70">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:11">
+      <c r="M70">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N70">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14">
       <c r="A71" t="s">
-        <v>81</v>
+        <v>85</v>
+      </c>
+      <c r="B71">
+        <v>1</v>
+      </c>
+      <c r="C71">
+        <v>1</v>
       </c>
       <c r="D71">
         <v>1</v>
@@ -2453,6 +3881,12 @@
       <c r="F71">
         <v>2</v>
       </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
       <c r="I71">
         <v>0</v>
       </c>
@@ -2462,10 +3896,24 @@
       <c r="K71">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:11">
+      <c r="M71">
+        <f t="shared" si="3"/>
+        <v>1.2</v>
+      </c>
+      <c r="N71">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14">
       <c r="A72" t="s">
-        <v>82</v>
+        <v>86</v>
+      </c>
+      <c r="B72">
+        <v>0</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
       </c>
       <c r="D72">
         <v>0</v>
@@ -2476,6 +3924,12 @@
       <c r="F72">
         <v>0</v>
       </c>
+      <c r="G72">
+        <v>1</v>
+      </c>
+      <c r="H72">
+        <v>1</v>
+      </c>
       <c r="I72">
         <v>1</v>
       </c>
@@ -2485,10 +3939,24 @@
       <c r="K72">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:11">
+      <c r="M72">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+      <c r="N72">
+        <f t="shared" si="2"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14">
       <c r="A73" t="s">
-        <v>83</v>
+        <v>87</v>
+      </c>
+      <c r="B73">
+        <v>1</v>
+      </c>
+      <c r="C73">
+        <v>1</v>
       </c>
       <c r="D73">
         <v>1</v>
@@ -2499,6 +3967,12 @@
       <c r="F73">
         <v>0</v>
       </c>
+      <c r="G73">
+        <v>1</v>
+      </c>
+      <c r="H73">
+        <v>1</v>
+      </c>
       <c r="I73">
         <v>1</v>
       </c>
@@ -2508,10 +3982,24 @@
       <c r="K73">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:11">
+      <c r="M73">
+        <f t="shared" si="3"/>
+        <v>0.8</v>
+      </c>
+      <c r="N73">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14">
       <c r="A74" t="s">
-        <v>84</v>
+        <v>88</v>
+      </c>
+      <c r="B74">
+        <v>0</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
       </c>
       <c r="D74">
         <v>0</v>
@@ -2522,6 +4010,12 @@
       <c r="F74">
         <v>0</v>
       </c>
+      <c r="G74">
+        <v>0</v>
+      </c>
+      <c r="H74">
+        <v>0</v>
+      </c>
       <c r="I74">
         <v>0</v>
       </c>
@@ -2531,10 +4025,24 @@
       <c r="K74">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:11">
+      <c r="M74">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N74">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14">
       <c r="A75" t="s">
-        <v>85</v>
+        <v>89</v>
+      </c>
+      <c r="B75">
+        <v>1</v>
+      </c>
+      <c r="C75">
+        <v>1</v>
       </c>
       <c r="D75">
         <v>1</v>
@@ -2545,6 +4053,12 @@
       <c r="F75">
         <v>1</v>
       </c>
+      <c r="G75">
+        <v>0</v>
+      </c>
+      <c r="H75">
+        <v>0</v>
+      </c>
       <c r="I75">
         <v>0</v>
       </c>
@@ -2554,10 +4068,24 @@
       <c r="K75">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:11">
+      <c r="M75">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="N75">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14">
       <c r="A76" t="s">
-        <v>86</v>
+        <v>90</v>
+      </c>
+      <c r="B76">
+        <v>0</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
       </c>
       <c r="D76">
         <v>0</v>
@@ -2568,6 +4096,12 @@
       <c r="F76">
         <v>0</v>
       </c>
+      <c r="G76">
+        <v>0</v>
+      </c>
+      <c r="H76">
+        <v>0</v>
+      </c>
       <c r="I76">
         <v>0</v>
       </c>
@@ -2577,10 +4111,24 @@
       <c r="K76">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:11">
+      <c r="M76">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N76">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14">
       <c r="A77" t="s">
-        <v>87</v>
+        <v>91</v>
+      </c>
+      <c r="B77">
+        <v>0</v>
+      </c>
+      <c r="C77">
+        <v>1</v>
       </c>
       <c r="D77">
         <v>1</v>
@@ -2591,6 +4139,12 @@
       <c r="F77">
         <v>0</v>
       </c>
+      <c r="G77">
+        <v>1</v>
+      </c>
+      <c r="H77">
+        <v>1</v>
+      </c>
       <c r="I77">
         <v>1</v>
       </c>
@@ -2600,10 +4154,24 @@
       <c r="K77">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="1:11">
+      <c r="M77">
+        <f t="shared" si="3"/>
+        <v>0.4</v>
+      </c>
+      <c r="N77">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14">
       <c r="A78" t="s">
-        <v>88</v>
+        <v>92</v>
+      </c>
+      <c r="B78">
+        <v>0</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
       </c>
       <c r="D78">
         <v>0</v>
@@ -2614,6 +4182,12 @@
       <c r="F78">
         <v>0</v>
       </c>
+      <c r="G78">
+        <v>0</v>
+      </c>
+      <c r="H78">
+        <v>0</v>
+      </c>
       <c r="I78">
         <v>0</v>
       </c>
@@ -2623,10 +4197,24 @@
       <c r="K78">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:11">
+      <c r="M78">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N78">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14">
       <c r="A79" t="s">
-        <v>89</v>
+        <v>93</v>
+      </c>
+      <c r="B79">
+        <v>0</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
       </c>
       <c r="D79">
         <v>1</v>
@@ -2637,6 +4225,12 @@
       <c r="F79">
         <v>0</v>
       </c>
+      <c r="G79">
+        <v>0</v>
+      </c>
+      <c r="H79">
+        <v>0</v>
+      </c>
       <c r="I79">
         <v>0</v>
       </c>
@@ -2646,10 +4240,24 @@
       <c r="K79">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:11">
+      <c r="M79">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+      <c r="N79">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14">
       <c r="A80" t="s">
-        <v>90</v>
+        <v>94</v>
+      </c>
+      <c r="B80">
+        <v>0</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
       </c>
       <c r="D80">
         <v>0</v>
@@ -2660,6 +4268,12 @@
       <c r="F80">
         <v>0</v>
       </c>
+      <c r="G80">
+        <v>0</v>
+      </c>
+      <c r="H80">
+        <v>0</v>
+      </c>
       <c r="I80">
         <v>0</v>
       </c>
@@ -2669,10 +4283,24 @@
       <c r="K80">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:11">
+      <c r="M80">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N80">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14">
       <c r="A81" t="s">
-        <v>91</v>
+        <v>95</v>
+      </c>
+      <c r="B81">
+        <v>1</v>
+      </c>
+      <c r="C81">
+        <v>1</v>
       </c>
       <c r="D81">
         <v>1</v>
@@ -2683,6 +4311,12 @@
       <c r="F81">
         <v>2</v>
       </c>
+      <c r="G81">
+        <v>0</v>
+      </c>
+      <c r="H81">
+        <v>0</v>
+      </c>
       <c r="I81">
         <v>0</v>
       </c>
@@ -2692,10 +4326,24 @@
       <c r="K81">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:11">
+      <c r="M81">
+        <f t="shared" si="3"/>
+        <v>1.2</v>
+      </c>
+      <c r="N81">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14">
       <c r="A82" t="s">
-        <v>92</v>
+        <v>96</v>
+      </c>
+      <c r="B82">
+        <v>0</v>
+      </c>
+      <c r="C82">
+        <v>0</v>
       </c>
       <c r="D82">
         <v>0</v>
@@ -2706,6 +4354,12 @@
       <c r="F82">
         <v>0</v>
       </c>
+      <c r="G82">
+        <v>0</v>
+      </c>
+      <c r="H82">
+        <v>0</v>
+      </c>
       <c r="I82">
         <v>0</v>
       </c>
@@ -2715,10 +4369,24 @@
       <c r="K82">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:11">
+      <c r="M82">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N82">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14">
       <c r="A83" t="s">
-        <v>93</v>
+        <v>97</v>
+      </c>
+      <c r="B83">
+        <v>3</v>
+      </c>
+      <c r="C83">
+        <v>3</v>
       </c>
       <c r="D83">
         <v>3</v>
@@ -2729,6 +4397,12 @@
       <c r="F83">
         <v>3</v>
       </c>
+      <c r="G83">
+        <v>0</v>
+      </c>
+      <c r="H83">
+        <v>0</v>
+      </c>
       <c r="I83">
         <v>0</v>
       </c>
@@ -2738,10 +4412,24 @@
       <c r="K83">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:11">
+      <c r="M83">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="N83">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14">
       <c r="A84" t="s">
-        <v>94</v>
+        <v>98</v>
+      </c>
+      <c r="B84">
+        <v>1</v>
+      </c>
+      <c r="C84">
+        <v>1</v>
       </c>
       <c r="D84">
         <v>1</v>
@@ -2752,6 +4440,12 @@
       <c r="F84">
         <v>1</v>
       </c>
+      <c r="G84">
+        <v>0</v>
+      </c>
+      <c r="H84">
+        <v>0</v>
+      </c>
       <c r="I84">
         <v>0</v>
       </c>
@@ -2761,10 +4455,24 @@
       <c r="K84">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:11">
+      <c r="M84">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="N84">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14">
       <c r="A85" t="s">
-        <v>95</v>
+        <v>99</v>
+      </c>
+      <c r="B85">
+        <v>0</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
       </c>
       <c r="D85">
         <v>0</v>
@@ -2775,6 +4483,12 @@
       <c r="F85">
         <v>0</v>
       </c>
+      <c r="G85">
+        <v>0</v>
+      </c>
+      <c r="H85">
+        <v>0</v>
+      </c>
       <c r="I85">
         <v>0</v>
       </c>
@@ -2784,10 +4498,24 @@
       <c r="K85">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:11">
+      <c r="M85">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N85">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14">
       <c r="A86" t="s">
-        <v>96</v>
+        <v>100</v>
+      </c>
+      <c r="B86">
+        <v>0</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
       </c>
       <c r="D86">
         <v>0</v>
@@ -2798,6 +4526,12 @@
       <c r="F86">
         <v>0</v>
       </c>
+      <c r="G86">
+        <v>0</v>
+      </c>
+      <c r="H86">
+        <v>1</v>
+      </c>
       <c r="I86">
         <v>0</v>
       </c>
@@ -2807,10 +4541,24 @@
       <c r="K86">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:11">
+      <c r="M86">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N86">
+        <f t="shared" si="2"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14">
       <c r="A87" t="s">
-        <v>97</v>
+        <v>101</v>
+      </c>
+      <c r="B87">
+        <v>2</v>
+      </c>
+      <c r="C87">
+        <v>2</v>
       </c>
       <c r="D87">
         <v>2</v>
@@ -2821,6 +4569,12 @@
       <c r="F87">
         <v>2</v>
       </c>
+      <c r="G87">
+        <v>0</v>
+      </c>
+      <c r="H87">
+        <v>0</v>
+      </c>
       <c r="I87">
         <v>0</v>
       </c>
@@ -2830,10 +4584,24 @@
       <c r="K87">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:11">
+      <c r="M87">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="N87">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14">
       <c r="A88" t="s">
-        <v>98</v>
+        <v>102</v>
+      </c>
+      <c r="B88">
+        <v>1</v>
+      </c>
+      <c r="C88">
+        <v>1</v>
       </c>
       <c r="D88">
         <v>0</v>
@@ -2844,6 +4612,12 @@
       <c r="F88">
         <v>1</v>
       </c>
+      <c r="G88">
+        <v>1</v>
+      </c>
+      <c r="H88">
+        <v>1</v>
+      </c>
       <c r="I88">
         <v>1</v>
       </c>
@@ -2853,10 +4627,24 @@
       <c r="K88">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:11">
+      <c r="M88">
+        <f t="shared" si="3"/>
+        <v>0.8</v>
+      </c>
+      <c r="N88">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14">
       <c r="A89" t="s">
-        <v>99</v>
+        <v>103</v>
+      </c>
+      <c r="B89">
+        <v>3</v>
+      </c>
+      <c r="C89">
+        <v>3</v>
       </c>
       <c r="D89">
         <v>3</v>
@@ -2867,6 +4655,12 @@
       <c r="F89">
         <v>3</v>
       </c>
+      <c r="G89">
+        <v>1</v>
+      </c>
+      <c r="H89">
+        <v>1</v>
+      </c>
       <c r="I89">
         <v>0</v>
       </c>
@@ -2876,10 +4670,24 @@
       <c r="K89">
         <v>1</v>
       </c>
-    </row>
-    <row r="90" spans="1:11">
+      <c r="M89">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="N89">
+        <f t="shared" si="2"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14">
       <c r="A90" t="s">
-        <v>100</v>
+        <v>104</v>
+      </c>
+      <c r="B90">
+        <v>0</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
       </c>
       <c r="D90">
         <v>0</v>
@@ -2890,6 +4698,12 @@
       <c r="F90">
         <v>0</v>
       </c>
+      <c r="G90">
+        <v>0</v>
+      </c>
+      <c r="H90">
+        <v>0</v>
+      </c>
       <c r="I90">
         <v>0</v>
       </c>
@@ -2899,10 +4713,24 @@
       <c r="K90">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:11">
+      <c r="M90">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N90">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14">
       <c r="A91" t="s">
-        <v>101</v>
+        <v>105</v>
+      </c>
+      <c r="B91">
+        <v>3</v>
+      </c>
+      <c r="C91">
+        <v>3</v>
       </c>
       <c r="D91">
         <v>3</v>
@@ -2913,6 +4741,12 @@
       <c r="F91">
         <v>3</v>
       </c>
+      <c r="G91">
+        <v>0</v>
+      </c>
+      <c r="H91">
+        <v>0</v>
+      </c>
       <c r="I91">
         <v>0</v>
       </c>
@@ -2922,10 +4756,24 @@
       <c r="K91">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:11">
+      <c r="M91">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="N91">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14">
       <c r="A92" t="s">
-        <v>102</v>
+        <v>106</v>
+      </c>
+      <c r="B92">
+        <v>3</v>
+      </c>
+      <c r="C92">
+        <v>3</v>
       </c>
       <c r="D92">
         <v>3</v>
@@ -2936,6 +4784,12 @@
       <c r="F92">
         <v>2</v>
       </c>
+      <c r="G92">
+        <v>0</v>
+      </c>
+      <c r="H92">
+        <v>0</v>
+      </c>
       <c r="I92">
         <v>0</v>
       </c>
@@ -2945,10 +4799,24 @@
       <c r="K92">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:11">
+      <c r="M92">
+        <f t="shared" si="3"/>
+        <v>2.8</v>
+      </c>
+      <c r="N92">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14">
       <c r="A93" t="s">
-        <v>103</v>
+        <v>107</v>
+      </c>
+      <c r="B93">
+        <v>3</v>
+      </c>
+      <c r="C93">
+        <v>3</v>
       </c>
       <c r="D93">
         <v>3</v>
@@ -2959,6 +4827,12 @@
       <c r="F93">
         <v>2</v>
       </c>
+      <c r="G93">
+        <v>1</v>
+      </c>
+      <c r="H93">
+        <v>1</v>
+      </c>
       <c r="I93">
         <v>1</v>
       </c>
@@ -2968,10 +4842,24 @@
       <c r="K93">
         <v>1</v>
       </c>
-    </row>
-    <row r="94" spans="1:11">
+      <c r="M93">
+        <f t="shared" si="3"/>
+        <v>2.8</v>
+      </c>
+      <c r="N93">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14">
       <c r="A94" t="s">
-        <v>104</v>
+        <v>108</v>
+      </c>
+      <c r="B94">
+        <v>0</v>
+      </c>
+      <c r="C94">
+        <v>0</v>
       </c>
       <c r="D94">
         <v>0</v>
@@ -2982,6 +4870,12 @@
       <c r="F94">
         <v>0</v>
       </c>
+      <c r="G94">
+        <v>0</v>
+      </c>
+      <c r="H94">
+        <v>0</v>
+      </c>
       <c r="I94">
         <v>0</v>
       </c>
@@ -2991,10 +4885,24 @@
       <c r="K94">
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:11">
+      <c r="M94">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N94">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14">
       <c r="A95" t="s">
-        <v>105</v>
+        <v>109</v>
+      </c>
+      <c r="B95">
+        <v>1</v>
+      </c>
+      <c r="C95">
+        <v>1</v>
       </c>
       <c r="D95">
         <v>1</v>
@@ -3005,6 +4913,12 @@
       <c r="F95">
         <v>0</v>
       </c>
+      <c r="G95">
+        <v>1</v>
+      </c>
+      <c r="H95">
+        <v>1</v>
+      </c>
       <c r="I95">
         <v>1</v>
       </c>
@@ -3014,10 +4928,24 @@
       <c r="K95">
         <v>1</v>
       </c>
-    </row>
-    <row r="96" spans="1:11">
+      <c r="M95">
+        <f t="shared" si="3"/>
+        <v>0.8</v>
+      </c>
+      <c r="N95">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14">
       <c r="A96" t="s">
-        <v>106</v>
+        <v>110</v>
+      </c>
+      <c r="B96">
+        <v>0</v>
+      </c>
+      <c r="C96">
+        <v>0</v>
       </c>
       <c r="D96">
         <v>0</v>
@@ -3028,6 +4956,12 @@
       <c r="F96">
         <v>0</v>
       </c>
+      <c r="G96">
+        <v>1</v>
+      </c>
+      <c r="H96">
+        <v>1</v>
+      </c>
       <c r="I96">
         <v>1</v>
       </c>
@@ -3037,10 +4971,24 @@
       <c r="K96">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="1:11">
+      <c r="M96">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+      <c r="N96">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14">
       <c r="A97" t="s">
-        <v>107</v>
+        <v>111</v>
+      </c>
+      <c r="B97">
+        <v>0</v>
+      </c>
+      <c r="C97">
+        <v>0</v>
       </c>
       <c r="D97">
         <v>0</v>
@@ -3051,6 +4999,12 @@
       <c r="F97">
         <v>0</v>
       </c>
+      <c r="G97">
+        <v>0</v>
+      </c>
+      <c r="H97">
+        <v>0</v>
+      </c>
       <c r="I97">
         <v>0</v>
       </c>
@@ -3060,10 +5014,24 @@
       <c r="K97">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:11">
+      <c r="M97">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+      <c r="N97">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14">
       <c r="A98" t="s">
-        <v>108</v>
+        <v>112</v>
+      </c>
+      <c r="B98">
+        <v>2</v>
+      </c>
+      <c r="C98">
+        <v>2</v>
       </c>
       <c r="D98">
         <v>2</v>
@@ -3074,6 +5042,12 @@
       <c r="F98">
         <v>3</v>
       </c>
+      <c r="G98">
+        <v>0</v>
+      </c>
+      <c r="H98">
+        <v>0</v>
+      </c>
       <c r="I98">
         <v>0</v>
       </c>
@@ -3083,10 +5057,24 @@
       <c r="K98">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:11">
+      <c r="M98">
+        <f t="shared" si="3"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="N98">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14">
       <c r="A99" t="s">
-        <v>109</v>
+        <v>113</v>
+      </c>
+      <c r="B99">
+        <v>3</v>
+      </c>
+      <c r="C99">
+        <v>3</v>
       </c>
       <c r="D99">
         <v>3</v>
@@ -3097,6 +5085,12 @@
       <c r="F99">
         <v>3</v>
       </c>
+      <c r="G99">
+        <v>0</v>
+      </c>
+      <c r="H99">
+        <v>0</v>
+      </c>
       <c r="I99">
         <v>0</v>
       </c>
@@ -3106,10 +5100,24 @@
       <c r="K99">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:11">
+      <c r="M99">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="N99">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14">
       <c r="A100" t="s">
-        <v>110</v>
+        <v>114</v>
+      </c>
+      <c r="B100">
+        <v>0</v>
+      </c>
+      <c r="C100">
+        <v>0</v>
       </c>
       <c r="D100">
         <v>0</v>
@@ -3120,6 +5128,12 @@
       <c r="F100">
         <v>0</v>
       </c>
+      <c r="G100">
+        <v>0</v>
+      </c>
+      <c r="H100">
+        <v>0</v>
+      </c>
       <c r="I100">
         <v>0</v>
       </c>
@@ -3129,10 +5143,24 @@
       <c r="K100">
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="1:11">
+      <c r="M100">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N100">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14">
       <c r="A101" t="s">
-        <v>111</v>
+        <v>115</v>
+      </c>
+      <c r="B101">
+        <v>1</v>
+      </c>
+      <c r="C101">
+        <v>1</v>
       </c>
       <c r="D101">
         <v>1</v>
@@ -3143,6 +5171,12 @@
       <c r="F101">
         <v>1</v>
       </c>
+      <c r="G101">
+        <v>0</v>
+      </c>
+      <c r="H101">
+        <v>0</v>
+      </c>
       <c r="I101">
         <v>0</v>
       </c>
@@ -3152,10 +5186,24 @@
       <c r="K101">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:11">
+      <c r="M101">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="N101">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14">
       <c r="A102" t="s">
-        <v>112</v>
+        <v>116</v>
+      </c>
+      <c r="B102">
+        <v>0</v>
+      </c>
+      <c r="C102">
+        <v>0</v>
       </c>
       <c r="D102">
         <v>0</v>
@@ -3166,6 +5214,12 @@
       <c r="F102">
         <v>0</v>
       </c>
+      <c r="G102">
+        <v>1</v>
+      </c>
+      <c r="H102">
+        <v>1</v>
+      </c>
       <c r="I102">
         <v>1</v>
       </c>
@@ -3175,10 +5229,24 @@
       <c r="K102">
         <v>1</v>
       </c>
-    </row>
-    <row r="103" spans="1:11">
+      <c r="M102">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N102">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14">
       <c r="A103" t="s">
-        <v>113</v>
+        <v>117</v>
+      </c>
+      <c r="B103">
+        <v>0</v>
+      </c>
+      <c r="C103">
+        <v>0</v>
       </c>
       <c r="D103">
         <v>0</v>
@@ -3189,6 +5257,12 @@
       <c r="F103">
         <v>0</v>
       </c>
+      <c r="G103">
+        <v>0</v>
+      </c>
+      <c r="H103">
+        <v>0</v>
+      </c>
       <c r="I103">
         <v>0</v>
       </c>
@@ -3198,10 +5272,24 @@
       <c r="K103">
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="1:11">
+      <c r="M103">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N103">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14">
       <c r="A104" t="s">
-        <v>114</v>
+        <v>118</v>
+      </c>
+      <c r="B104">
+        <v>2</v>
+      </c>
+      <c r="C104">
+        <v>2</v>
       </c>
       <c r="D104">
         <v>2</v>
@@ -3212,6 +5300,12 @@
       <c r="F104">
         <v>2</v>
       </c>
+      <c r="G104">
+        <v>0</v>
+      </c>
+      <c r="H104">
+        <v>0</v>
+      </c>
       <c r="I104">
         <v>0</v>
       </c>
@@ -3221,10 +5315,24 @@
       <c r="K104">
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:11">
+      <c r="M104">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="N104">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14">
       <c r="A105" t="s">
-        <v>115</v>
+        <v>119</v>
+      </c>
+      <c r="B105">
+        <v>0</v>
+      </c>
+      <c r="C105">
+        <v>0</v>
       </c>
       <c r="D105">
         <v>0</v>
@@ -3235,6 +5343,12 @@
       <c r="F105">
         <v>0</v>
       </c>
+      <c r="G105">
+        <v>0</v>
+      </c>
+      <c r="H105">
+        <v>0</v>
+      </c>
       <c r="I105">
         <v>0</v>
       </c>
@@ -3244,10 +5358,24 @@
       <c r="K105">
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="1:11">
+      <c r="M105">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N105">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14">
       <c r="A106" t="s">
-        <v>116</v>
+        <v>120</v>
+      </c>
+      <c r="B106">
+        <v>1</v>
+      </c>
+      <c r="C106">
+        <v>1</v>
       </c>
       <c r="D106">
         <v>1</v>
@@ -3258,6 +5386,12 @@
       <c r="F106">
         <v>0</v>
       </c>
+      <c r="G106">
+        <v>1</v>
+      </c>
+      <c r="H106">
+        <v>1</v>
+      </c>
       <c r="I106">
         <v>1</v>
       </c>
@@ -3267,10 +5401,24 @@
       <c r="K106">
         <v>1</v>
       </c>
-    </row>
-    <row r="107" spans="1:11">
+      <c r="M106">
+        <f t="shared" si="3"/>
+        <v>0.8</v>
+      </c>
+      <c r="N106">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14">
       <c r="A107" t="s">
-        <v>117</v>
+        <v>121</v>
+      </c>
+      <c r="B107">
+        <v>3</v>
+      </c>
+      <c r="C107">
+        <v>3</v>
       </c>
       <c r="D107">
         <v>3</v>
@@ -3281,6 +5429,12 @@
       <c r="F107">
         <v>3</v>
       </c>
+      <c r="G107">
+        <v>0</v>
+      </c>
+      <c r="H107">
+        <v>0</v>
+      </c>
       <c r="I107">
         <v>0</v>
       </c>
@@ -3290,10 +5444,24 @@
       <c r="K107">
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="1:11">
+      <c r="M107">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="N107">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14">
       <c r="A108" t="s">
-        <v>118</v>
+        <v>122</v>
+      </c>
+      <c r="B108">
+        <v>1</v>
+      </c>
+      <c r="C108">
+        <v>1</v>
       </c>
       <c r="D108">
         <v>1</v>
@@ -3304,6 +5472,12 @@
       <c r="F108">
         <v>1</v>
       </c>
+      <c r="G108">
+        <v>0</v>
+      </c>
+      <c r="H108">
+        <v>0</v>
+      </c>
       <c r="I108">
         <v>0</v>
       </c>
@@ -3313,10 +5487,24 @@
       <c r="K108">
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="1:11">
+      <c r="M108">
+        <f t="shared" si="3"/>
+        <v>1.2</v>
+      </c>
+      <c r="N108">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:14">
       <c r="A109" t="s">
-        <v>119</v>
+        <v>123</v>
+      </c>
+      <c r="B109">
+        <v>0</v>
+      </c>
+      <c r="C109">
+        <v>0</v>
       </c>
       <c r="D109">
         <v>0</v>
@@ -3327,6 +5515,12 @@
       <c r="F109">
         <v>0</v>
       </c>
+      <c r="G109">
+        <v>0</v>
+      </c>
+      <c r="H109">
+        <v>0</v>
+      </c>
       <c r="I109">
         <v>0</v>
       </c>
@@ -3336,10 +5530,24 @@
       <c r="K109">
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="1:11">
+      <c r="M109">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N109">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14">
       <c r="A110" t="s">
-        <v>120</v>
+        <v>124</v>
+      </c>
+      <c r="B110">
+        <v>3</v>
+      </c>
+      <c r="C110">
+        <v>2</v>
       </c>
       <c r="D110">
         <v>3</v>
@@ -3350,6 +5558,12 @@
       <c r="F110">
         <v>2</v>
       </c>
+      <c r="G110">
+        <v>1</v>
+      </c>
+      <c r="H110">
+        <v>1</v>
+      </c>
       <c r="I110">
         <v>1</v>
       </c>
@@ -3359,10 +5573,24 @@
       <c r="K110">
         <v>1</v>
       </c>
-    </row>
-    <row r="111" spans="1:11">
+      <c r="M110">
+        <f t="shared" si="3"/>
+        <v>2.6</v>
+      </c>
+      <c r="N110">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:14">
       <c r="A111" t="s">
-        <v>121</v>
+        <v>125</v>
+      </c>
+      <c r="B111">
+        <v>0</v>
+      </c>
+      <c r="C111">
+        <v>0</v>
       </c>
       <c r="D111">
         <v>0</v>
@@ -3373,6 +5601,12 @@
       <c r="F111">
         <v>0</v>
       </c>
+      <c r="G111">
+        <v>0</v>
+      </c>
+      <c r="H111">
+        <v>0</v>
+      </c>
       <c r="I111">
         <v>0</v>
       </c>
@@ -3382,10 +5616,24 @@
       <c r="K111">
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="1:11">
+      <c r="M111">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N111">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:14">
       <c r="A112" t="s">
-        <v>122</v>
+        <v>126</v>
+      </c>
+      <c r="B112">
+        <v>2</v>
+      </c>
+      <c r="C112">
+        <v>2</v>
       </c>
       <c r="D112">
         <v>3</v>
@@ -3396,6 +5644,12 @@
       <c r="F112">
         <v>2</v>
       </c>
+      <c r="G112">
+        <v>1</v>
+      </c>
+      <c r="H112">
+        <v>1</v>
+      </c>
       <c r="I112">
         <v>1</v>
       </c>
@@ -3405,10 +5659,24 @@
       <c r="K112">
         <v>1</v>
       </c>
-    </row>
-    <row r="113" spans="1:11">
+      <c r="M112">
+        <f t="shared" si="3"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="N112">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:14">
       <c r="A113" t="s">
-        <v>123</v>
+        <v>127</v>
+      </c>
+      <c r="B113">
+        <v>0</v>
+      </c>
+      <c r="C113">
+        <v>0</v>
       </c>
       <c r="D113">
         <v>0</v>
@@ -3419,6 +5687,12 @@
       <c r="F113">
         <v>0</v>
       </c>
+      <c r="G113">
+        <v>1</v>
+      </c>
+      <c r="H113">
+        <v>1</v>
+      </c>
       <c r="I113">
         <v>1</v>
       </c>
@@ -3428,10 +5702,24 @@
       <c r="K113">
         <v>1</v>
       </c>
-    </row>
-    <row r="114" spans="1:11">
+      <c r="M113">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N113">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:14">
       <c r="A114" t="s">
-        <v>124</v>
+        <v>128</v>
+      </c>
+      <c r="B114">
+        <v>3</v>
+      </c>
+      <c r="C114">
+        <v>3</v>
       </c>
       <c r="D114">
         <v>3</v>
@@ -3442,6 +5730,12 @@
       <c r="F114">
         <v>3</v>
       </c>
+      <c r="G114">
+        <v>0</v>
+      </c>
+      <c r="H114">
+        <v>0</v>
+      </c>
       <c r="I114">
         <v>0</v>
       </c>
@@ -3451,10 +5745,24 @@
       <c r="K114">
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="1:11">
+      <c r="M114">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="N114">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:14">
       <c r="A115" t="s">
-        <v>125</v>
+        <v>129</v>
+      </c>
+      <c r="B115">
+        <v>3</v>
+      </c>
+      <c r="C115">
+        <v>3</v>
       </c>
       <c r="D115">
         <v>3</v>
@@ -3465,6 +5773,12 @@
       <c r="F115">
         <v>3</v>
       </c>
+      <c r="G115">
+        <v>0</v>
+      </c>
+      <c r="H115">
+        <v>0</v>
+      </c>
       <c r="I115">
         <v>0</v>
       </c>
@@ -3474,10 +5788,24 @@
       <c r="K115">
         <v>0</v>
       </c>
-    </row>
-    <row r="116" spans="1:11">
+      <c r="M115">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="N115">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14">
       <c r="A116" t="s">
-        <v>126</v>
+        <v>130</v>
+      </c>
+      <c r="B116">
+        <v>0</v>
+      </c>
+      <c r="C116">
+        <v>0</v>
       </c>
       <c r="D116">
         <v>0</v>
@@ -3488,6 +5816,12 @@
       <c r="F116">
         <v>0</v>
       </c>
+      <c r="G116">
+        <v>1</v>
+      </c>
+      <c r="H116">
+        <v>1</v>
+      </c>
       <c r="I116">
         <v>1</v>
       </c>
@@ -3497,10 +5831,24 @@
       <c r="K116">
         <v>1</v>
       </c>
-    </row>
-    <row r="117" spans="1:11">
+      <c r="M116">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N116">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:14">
       <c r="A117" t="s">
-        <v>127</v>
+        <v>131</v>
+      </c>
+      <c r="B117">
+        <v>2</v>
+      </c>
+      <c r="C117">
+        <v>2</v>
       </c>
       <c r="D117">
         <v>2</v>
@@ -3511,6 +5859,12 @@
       <c r="F117">
         <v>1</v>
       </c>
+      <c r="G117">
+        <v>1</v>
+      </c>
+      <c r="H117">
+        <v>1</v>
+      </c>
       <c r="I117">
         <v>1</v>
       </c>
@@ -3520,10 +5874,24 @@
       <c r="K117">
         <v>1</v>
       </c>
-    </row>
-    <row r="118" spans="1:11">
+      <c r="M117">
+        <f t="shared" si="3"/>
+        <v>1.8</v>
+      </c>
+      <c r="N117">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:14">
       <c r="A118" t="s">
-        <v>128</v>
+        <v>132</v>
+      </c>
+      <c r="B118">
+        <v>2</v>
+      </c>
+      <c r="C118">
+        <v>2</v>
       </c>
       <c r="D118">
         <v>2</v>
@@ -3534,6 +5902,12 @@
       <c r="F118">
         <v>2</v>
       </c>
+      <c r="G118">
+        <v>0</v>
+      </c>
+      <c r="H118">
+        <v>0</v>
+      </c>
       <c r="I118">
         <v>0</v>
       </c>
@@ -3542,6 +5916,27 @@
       </c>
       <c r="K118">
         <v>0</v>
+      </c>
+      <c r="M118">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="N118">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:14">
+      <c r="L119" t="s">
+        <v>133</v>
+      </c>
+      <c r="M119" s="1">
+        <f>ROUND(AVERAGE(M2:M118),2)</f>
+        <v>1.03</v>
+      </c>
+      <c r="N119" s="2">
+        <f>ROUND(AVERAGE(N2:N118),2)</f>
+        <v>0.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>